<commit_message>
Actualizo el presupuesto y consumo.
</commit_message>
<xml_diff>
--- a/CABLEADO ESTRUCTURADO/Consumo.xlsx
+++ b/CABLEADO ESTRUCTURADO/Consumo.xlsx
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,14 +1157,14 @@
         <v>3</v>
       </c>
       <c r="D31" s="7">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E31" s="7">
         <v>400</v>
       </c>
       <c r="F31" s="7">
         <f t="shared" ref="F31" si="4">D31*E31</f>
-        <v>3600</v>
+        <v>5600</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>3</v>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="F34" s="7">
         <f>SUM(F30:F33)</f>
-        <v>4035</v>
+        <v>6035</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>12</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="F35" s="15">
         <f>F34+(F34*$I$41)</f>
-        <v>4842</v>
+        <v>7242</v>
       </c>
       <c r="K35" s="14" t="s">
         <v>17</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="F36" s="26">
         <f>F35/$L$41</f>
-        <v>22.009090909090908</v>
+        <v>32.918181818181822</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>20</v>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="I42">
         <f>F13+L10+F23+L23+F35+L35+F48+F57+L57</f>
-        <v>47006.400000000009</v>
+        <v>49406.400000000009</v>
       </c>
       <c r="J42" t="s">
         <v>15</v>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="I44" s="12">
         <f>I42/L41</f>
-        <v>213.66545454545459</v>
+        <v>224.5745454545455</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizo el presupuesto y consumo. Subo el cableado de red del 3º, 4º y 5º piso y del edificio de Producción y Expedición.
</commit_message>
<xml_diff>
--- a/CABLEADO ESTRUCTURADO/Consumo.xlsx
+++ b/CABLEADO ESTRUCTURADO/Consumo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="34">
   <si>
     <t>Planta Baja</t>
   </si>
@@ -117,16 +117,7 @@
     <t>Switch fibra</t>
   </si>
   <si>
-    <t>0,85*</t>
-  </si>
-  <si>
-    <t>Pot Transf.(KV)</t>
-  </si>
-  <si>
-    <t>Transf (KVA)</t>
-  </si>
-  <si>
-    <t>Factor utliz.(%)</t>
+    <t>Produccion - Expedición</t>
   </si>
 </sst>
 </file>
@@ -256,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -313,7 +304,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1335,8 +1325,8 @@
         <v>14</v>
       </c>
       <c r="I42">
-        <f>F13+L10+F23+L23+F35+L35+F47+F57+L57</f>
-        <v>49364.400000000009</v>
+        <f>F13+L10+F23+L23+F35+L35+F48+F57+L57</f>
+        <v>49406.400000000009</v>
       </c>
       <c r="J42" t="s">
         <v>15</v>
@@ -1359,7 +1349,7 @@
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -1376,66 +1366,58 @@
       </c>
       <c r="I44" s="12">
         <f>I42/L41</f>
-        <v>224.38363636363641</v>
+        <v>224.5745454545455</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C45" s="4"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="C45" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7">
+        <v>35</v>
+      </c>
+      <c r="F45" s="7">
+        <f>D45*E45</f>
+        <v>35</v>
+      </c>
       <c r="M45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E46" s="4" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E47" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="7">
-        <f>SUM(F42:F45)</f>
-        <v>935</v>
-      </c>
-      <c r="K46" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E47" s="14" t="s">
+      <c r="F47" s="7">
+        <f>SUM(F42:F46)</f>
+        <v>970</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E48" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="15">
-        <f>F46+(F46*$I$41)</f>
-        <v>1122</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I47" s="30">
-        <f>I42/(0.85*1000)</f>
-        <v>58.075764705882364</v>
-      </c>
-      <c r="K47">
-        <v>75</v>
-      </c>
-      <c r="M47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="15">
+        <f>F47+(F47*$I$41)</f>
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F48" s="26">
-        <f>F47/$L$41</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I48" s="30">
-        <f>I47*100/(K47)</f>
-        <v>77.434352941176485</v>
+      <c r="F49" s="26">
+        <f>F48/$L$41</f>
+        <v>5.290909090909091</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agrego el informe de cableado estructurado. Actualizo Consumo.xlsx y PRESUPUESTO.xlsx. Agrego PDFs con las plantas.
</commit_message>
<xml_diff>
--- a/CABLEADO ESTRUCTURADO/Consumo.xlsx
+++ b/CABLEADO ESTRUCTURADO/Consumo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="270" windowWidth="20115" windowHeight="7875"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="40">
   <si>
     <t>Planta Baja</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Cable a usar(mm)</t>
+  </si>
+  <si>
+    <t>Modem Router</t>
   </si>
 </sst>
 </file>
@@ -694,18 +697,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59:G63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -790,14 +798,14 @@
         <v>3</v>
       </c>
       <c r="D5" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" s="7">
         <v>400</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F7" si="0">D5*E5</f>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>3</v>
@@ -815,7 +823,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -951,7 +959,7 @@
       </c>
       <c r="F12" s="24">
         <f>SUM(F4:F11)</f>
-        <v>7204</v>
+        <v>5204</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -960,7 +968,7 @@
       </c>
       <c r="F13" s="12">
         <f>F12+(F12*D54)</f>
-        <v>8644.7999999999993</v>
+        <v>6244.8</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -969,7 +977,7 @@
       </c>
       <c r="F14" s="22">
         <f>F13/$G$54</f>
-        <v>39.29454545454545</v>
+        <v>28.385454545454547</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -1460,7 +1468,7 @@
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -1484,19 +1492,10 @@
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="7">
-        <v>1</v>
-      </c>
-      <c r="E45" s="7">
-        <v>35</v>
-      </c>
-      <c r="F45" s="7">
-        <f>D45*E45</f>
-        <v>35</v>
-      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
       <c r="H45" s="16"/>
       <c r="I45" s="19"/>
       <c r="J45" s="18"/>
@@ -1509,10 +1508,13 @@
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C46" s="4"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="7">
+        <f>SUM(F42:F45)</f>
+        <v>935</v>
+      </c>
       <c r="K46" s="4" t="s">
         <v>19</v>
       </c>
@@ -1522,21 +1524,21 @@
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E47" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="7">
-        <f>SUM(F42:F46)</f>
-        <v>970</v>
+      <c r="E47" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="12">
+        <f>F46+(F46*$D$54)</f>
+        <v>1122</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E48" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="12">
-        <f>F47+(F47*$D$54)</f>
-        <v>1164</v>
+      <c r="E48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="22">
+        <f>F47/$G$54</f>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>1</v>
@@ -1547,13 +1549,6 @@
       <c r="J48" s="3"/>
     </row>
     <row r="49" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E49" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="22">
-        <f>F48/$G$54</f>
-        <v>5.290909090909091</v>
-      </c>
       <c r="H49" s="4" t="s">
         <v>2</v>
       </c>
@@ -1647,8 +1642,8 @@
         <v>14</v>
       </c>
       <c r="D55" s="36">
-        <f>F13+L10+F23+L23+F35+L35+F48+L45+L53</f>
-        <v>49406.400000000009</v>
+        <f>F13+L10+F23+L23+F35+L35+F47+L45+L53</f>
+        <v>46964.400000000009</v>
       </c>
       <c r="E55" s="37" t="s">
         <v>15</v>
@@ -1668,7 +1663,7 @@
       </c>
       <c r="D57" s="30">
         <f>D55/G54</f>
-        <v>224.5745454545455</v>
+        <v>213.47454545454551</v>
       </c>
       <c r="F57" s="40" t="s">
         <v>38</v>
@@ -1687,7 +1682,7 @@
       </c>
       <c r="I58">
         <f>D55*I56</f>
-        <v>40513.248000000007</v>
+        <v>38510.808000000005</v>
       </c>
     </row>
     <row r="59" spans="3:12" x14ac:dyDescent="0.25">

</xml_diff>